<commit_message>
try again fro Jenkins
</commit_message>
<xml_diff>
--- a/Alibaba/data/writeback.xlsx
+++ b/Alibaba/data/writeback.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="3">
   <si>
     <t>grape juice</t>
   </si>
@@ -65,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B130"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -672,6 +672,51 @@
         <v>2</v>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
add . to /target/...
</commit_message>
<xml_diff>
--- a/Alibaba/data/writeback.xlsx
+++ b/Alibaba/data/writeback.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="3">
   <si>
     <t>grape juice</t>
   </si>
@@ -65,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B130"/>
+  <dimension ref="A1:B133"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -717,6 +717,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>